<commit_message>
Updated to contributions data with 05-31-2024
</commit_message>
<xml_diff>
--- a/contributions.xlsx
+++ b/contributions.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5831" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5964" uniqueCount="1234">
   <si>
     <t>Person</t>
   </si>
@@ -3447,6 +3447,102 @@
     <t>https://github.com/asastats/channel/issues/986</t>
   </si>
   <si>
+    <t>Period below: 2024-4-07 to 2024-05-03 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period</t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/967</t>
+  </si>
+  <si>
+    <t>Grinnmarr</t>
+  </si>
+  <si>
+    <t>Blessed4aDay</t>
+  </si>
+  <si>
+    <t>uberg33k</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/910524302531649566/1228453068195102780</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/910524302531649566/1230282040868339873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motuwagon </t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/1001</t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/1002</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/1009792719897505912/1230941873657352203</t>
+  </si>
+  <si>
+    <t>ASA Stats DAO staking results tweet.</t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/discussions/1004</t>
+  </si>
+  <si>
+    <t>Period below: 2024-5-04 to 2024-05-31 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/908054304332603402/1238549968193585203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dankster1 </t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/1008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algoworm </t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/1028021510453084161/1243747790140735568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fifthrace </t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/1012</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/1009792719897505912/1240600152746623058</t>
+  </si>
+  <si>
+    <t>Group of recent Twitter replies</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/1009792719897505912/1240698847316148274</t>
+  </si>
+  <si>
+    <t>Governance reminder tweet</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/906917846754418770/1009792719897505912/1244951240916598815</t>
+  </si>
+  <si>
+    <t>Governance retweet</t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/issues/1003</t>
+  </si>
+  <si>
+    <t>akpepe</t>
+  </si>
+  <si>
+    <t>leaf 🍃</t>
+  </si>
+  <si>
+    <t>https://github.com/asastats/channel/discussions/1014</t>
+  </si>
+  <si>
     <t>Period below: 2023-12-16 to 2024-01-12 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period</t>
   </si>
   <si>
@@ -3727,6 +3823,12 @@
   </si>
   <si>
     <t>2024-04-06 Total</t>
+  </si>
+  <si>
+    <t>2024-05-03 Total</t>
+  </si>
+  <si>
+    <t>2024-05-31 Total</t>
   </si>
   <si>
     <t>Legal entity research Total</t>
@@ -4352,7 +4454,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:J1057" sheet="Ongoing Contributions"/>
+    <worksheetSource ref="A2:J1091" sheet="Ongoing Contributions"/>
   </cacheSource>
   <cacheFields>
     <cacheField name="Person" numFmtId="0">
@@ -4534,6 +4636,18 @@
         <s v="Period below: 2024-3-09 to 2024-04-06 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period"/>
         <s v="albino "/>
         <s v="DingusMungus "/>
+        <s v="Period below: 2024-4-07 to 2024-05-03 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period"/>
+        <s v="Grinnmarr"/>
+        <s v="Blessed4aDay"/>
+        <s v="uberg33k"/>
+        <s v="motuwagon "/>
+        <s v="Period below: 2024-5-04 to 2024-05-31 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period"/>
+        <s v="Max"/>
+        <s v="dankster1 "/>
+        <s v="Algoworm "/>
+        <s v="fifthrace "/>
+        <s v="akpepe"/>
+        <s v="leaf 🍃"/>
         <s v="Period below: 2023-12-16 to 2024-01-12 - Contribution list based on AlgoRhythMatic's sort of Github issues from this period"/>
         <s v="leaf "/>
         <s v="RandomTask "/>
@@ -4565,6 +4679,8 @@
         <d v="2024-01-13T00:00:00Z"/>
         <d v="2024-02-10T00:00:00Z"/>
         <d v="2024-03-09T00:00:00Z"/>
+        <d v="2024-04-07T00:00:00Z"/>
+        <d v="2024-05-04T00:00:00Z"/>
         <n v="45276.0"/>
       </sharedItems>
     </cacheField>
@@ -4595,6 +4711,8 @@
         <d v="2024-02-09T00:00:00Z"/>
         <d v="2024-03-08T00:00:00Z"/>
         <d v="2024-04-06T00:00:00Z"/>
+        <d v="2024-05-03T00:00:00Z"/>
+        <d v="2024-05-31T00:00:00Z"/>
         <n v="45303.0"/>
       </sharedItems>
     </cacheField>
@@ -5307,6 +5425,22 @@
         <s v="https://discord.com/channels/906917846754418770/908054330265960478/1225110783613079592"/>
         <s v="https://discord.com/channels/906917846754418770/908054330265960478/1225627979414241360"/>
         <s v="https://github.com/asastats/channel/issues/986"/>
+        <s v="https://github.com/asastats/channel/issues/967"/>
+        <s v="https://discord.com/channels/906917846754418770/910524302531649566/1228453068195102780"/>
+        <s v="https://discord.com/channels/906917846754418770/910524302531649566/1230282040868339873"/>
+        <s v="https://github.com/asastats/channel/issues/1001"/>
+        <s v="https://github.com/asastats/channel/issues/1002"/>
+        <s v="https://discord.com/channels/906917846754418770/1009792719897505912/1230941873657352203"/>
+        <s v="https://github.com/asastats/channel/discussions/1004"/>
+        <s v="https://discord.com/channels/906917846754418770/908054304332603402/1238549968193585203"/>
+        <s v="https://github.com/asastats/channel/issues/1008"/>
+        <s v="https://discord.com/channels/906917846754418770/1028021510453084161/1243747790140735568"/>
+        <s v="https://github.com/asastats/channel/issues/1012"/>
+        <s v="https://discord.com/channels/906917846754418770/1009792719897505912/1240600152746623058"/>
+        <s v="https://discord.com/channels/906917846754418770/1009792719897505912/1240698847316148274"/>
+        <s v="https://discord.com/channels/906917846754418770/1009792719897505912/1244951240916598815"/>
+        <s v="https://github.com/asastats/channel/issues/1003"/>
+        <s v="https://github.com/asastats/channel/discussions/1014"/>
         <s v="https://github.com/asastats/channel/issues/889"/>
         <s v="https://github.com/asastats/channel/issues/891"/>
         <s v="https://github.com/asastats/channel/issues/895"/>
@@ -5431,7 +5565,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Rewards by Period" cacheId="0" dataCaption="" createdVersion="6" compact="0" compactData="0">
-  <location ref="A1:C375" firstHeaderRow="0" firstDataRow="2" firstDataCol="0"/>
+  <location ref="A1:C398" firstHeaderRow="0" firstDataRow="2" firstDataCol="0"/>
   <pivotFields>
     <pivotField name="Person" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
       <items>
@@ -5477,9 +5611,11 @@
         <item x="21"/>
         <item x="22"/>
         <item x="97"/>
+        <item x="187"/>
         <item x="175"/>
         <item x="51"/>
         <item x="115"/>
+        <item x="185"/>
         <item x="36"/>
         <item x="75"/>
         <item x="41"/>
@@ -5487,6 +5623,7 @@
         <item x="98"/>
         <item x="91"/>
         <item x="55"/>
+        <item x="179"/>
         <item x="130"/>
         <item x="61"/>
         <item x="38"/>
@@ -5495,6 +5632,7 @@
         <item x="43"/>
         <item x="89"/>
         <item x="35"/>
+        <item x="184"/>
         <item x="138"/>
         <item x="176"/>
         <item x="151"/>
@@ -5502,9 +5640,11 @@
         <item x="66"/>
         <item x="141"/>
         <item x="37"/>
+        <item x="186"/>
         <item x="104"/>
         <item x="152"/>
         <item x="164"/>
+        <item x="178"/>
         <item x="172"/>
         <item x="168"/>
         <item x="46"/>
@@ -5514,9 +5654,11 @@
         <item x="144"/>
         <item x="48"/>
         <item x="72"/>
-        <item x="178"/>
+        <item x="190"/>
+        <item x="188"/>
         <item x="90"/>
         <item x="56"/>
+        <item x="183"/>
         <item x="150"/>
         <item x="163"/>
         <item x="82"/>
@@ -5532,6 +5674,7 @@
         <item x="34"/>
         <item x="80"/>
         <item x="63"/>
+        <item x="181"/>
         <item x="166"/>
         <item x="120"/>
         <item x="79"/>
@@ -5559,10 +5702,12 @@
         <item x="147"/>
         <item x="154"/>
         <item x="156"/>
-        <item x="177"/>
+        <item x="189"/>
         <item x="170"/>
         <item x="171"/>
         <item x="174"/>
+        <item x="177"/>
+        <item x="182"/>
         <item x="24"/>
         <item x="78"/>
         <item x="71"/>
@@ -5572,7 +5717,7 @@
         <item x="87"/>
         <item x="157"/>
         <item x="69"/>
-        <item x="179"/>
+        <item x="191"/>
         <item x="105"/>
         <item x="124"/>
         <item x="139"/>
@@ -5605,6 +5750,7 @@
         <item x="60"/>
         <item x="52"/>
         <item x="40"/>
+        <item x="180"/>
         <item x="123"/>
         <item x="158"/>
         <item x="53"/>
@@ -5645,6 +5791,8 @@
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5671,10 +5819,12 @@
         <item x="19"/>
         <item x="20"/>
         <item x="21"/>
-        <item x="25"/>
+        <item x="27"/>
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
         <item x="2"/>
         <item t="default"/>
       </items>
@@ -6428,6 +6578,22 @@
         <item x="712"/>
         <item x="713"/>
         <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="724"/>
+        <item x="725"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -50083,118 +50249,118 @@
       <c r="AC989" s="27"/>
     </row>
     <row r="990">
-      <c r="A990" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B990" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C990" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D990" s="5" t="s">
+      <c r="A990" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B990" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C990" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D990" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F990" s="54" t="s">
+      <c r="F990" s="10" t="s">
         <v>1116</v>
       </c>
-      <c r="G990" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H990" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I990" s="5">
+      <c r="G990" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H990" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I990" s="32">
         <v>1.0</v>
       </c>
       <c r="J990" s="5">
         <f>VLOOKUP(G990,rewardsModel,IFS(H990=1,2,H990=2,3,H990=3,4),false)*I990</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B991" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C991" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D991" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F991" s="54" t="s">
+      <c r="A991" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B991" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C991" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D991" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F991" s="10" t="s">
         <v>1116</v>
       </c>
-      <c r="G991" s="5" t="s">
+      <c r="G991" s="3" t="s">
         <v>91</v>
       </c>
       <c r="H991" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I991" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I991" s="32">
         <v>1.0</v>
       </c>
       <c r="J991" s="5">
         <f>VLOOKUP(G991,rewardsModel,IFS(H991=1,2,H991=2,3,H991=3,4),false)*I991</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B992" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C992" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D992" s="5" t="s">
+      <c r="A992" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B992" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C992" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D992" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F992" s="54" t="s">
-        <v>1117</v>
-      </c>
-      <c r="G992" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H992" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I992" s="5">
+      <c r="F992" s="10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G992" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H992" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I992" s="32">
         <v>1.0</v>
       </c>
       <c r="J992" s="5">
         <f>VLOOKUP(G992,rewardsModel,IFS(H992=1,2,H992=2,3,H992=3,4),false)*I992</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B993" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C993" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D993" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F993" s="54" t="s">
-        <v>1117</v>
-      </c>
-      <c r="G993" s="5" t="s">
+      <c r="A993" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B993" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C993" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D993" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F993" s="10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G993" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="H993" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I993" s="5">
+      <c r="H993" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I993" s="32">
         <v>1.0</v>
       </c>
       <c r="J993" s="5">
@@ -50203,28 +50369,28 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B994" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C994" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D994" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F994" s="54" t="s">
-        <v>1118</v>
-      </c>
-      <c r="G994" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H994" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I994" s="5">
+      <c r="A994" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="B994" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C994" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D994" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F994" s="10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G994" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H994" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I994" s="32">
         <v>1.0</v>
       </c>
       <c r="J994" s="5">
@@ -50233,28 +50399,28 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B995" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C995" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D995" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F995" s="54" t="s">
-        <v>1118</v>
-      </c>
-      <c r="G995" s="5" t="s">
+      <c r="A995" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B995" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C995" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D995" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F995" s="10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G995" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="H995" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I995" s="5">
+      <c r="H995" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I995" s="32">
         <v>1.0</v>
       </c>
       <c r="J995" s="5">
@@ -50263,58 +50429,58 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B996" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C996" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D996" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F996" s="54" t="s">
+      <c r="A996" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="G996" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H996" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I996" s="5">
+      <c r="B996" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C996" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D996" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F996" s="10" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G996" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H996" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I996" s="32">
         <v>1.0</v>
       </c>
       <c r="J996" s="5">
         <f>VLOOKUP(G996,rewardsModel,IFS(H996=1,2,H996=2,3,H996=3,4),false)*I996</f>
-        <v>0.03</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B997" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C997" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D997" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F997" s="54" t="s">
-        <v>1119</v>
-      </c>
-      <c r="G997" s="5" t="s">
+      <c r="A997" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B997" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C997" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D997" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F997" s="10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G997" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="H997" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I997" s="5">
+      <c r="H997" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I997" s="32">
         <v>1.0</v>
       </c>
       <c r="J997" s="5">
@@ -50323,28 +50489,28 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B998" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C998" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D998" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F998" s="54" t="s">
-        <v>1120</v>
-      </c>
-      <c r="G998" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H998" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I998" s="5">
+      <c r="A998" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B998" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C998" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D998" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F998" s="10" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G998" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H998" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I998" s="32">
         <v>1.0</v>
       </c>
       <c r="J998" s="5">
@@ -50353,28 +50519,28 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B999" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C999" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D999" s="5" t="s">
+      <c r="A999" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="B999" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C999" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D999" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F999" s="54" t="s">
-        <v>1120</v>
-      </c>
-      <c r="G999" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H999" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I999" s="5">
+      <c r="F999" s="10" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G999" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H999" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I999" s="32">
         <v>1.0</v>
       </c>
       <c r="J999" s="5">
@@ -50383,28 +50549,28 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1000" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1000" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1000" s="5" t="s">
+      <c r="A1000" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="B1000" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C1000" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D1000" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1000" s="54" t="s">
-        <v>1121</v>
-      </c>
-      <c r="G1000" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1000" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1000" s="5">
+      <c r="F1000" s="10" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G1000" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1000" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1000" s="32">
         <v>1.0</v>
       </c>
       <c r="J1000" s="5">
@@ -50413,148 +50579,127 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1001" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1001" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1001" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1001" s="54" t="s">
-        <v>1121</v>
-      </c>
-      <c r="G1001" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1001" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1001" s="5">
+      <c r="A1001" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1001" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C1001" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D1001" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1001" s="10" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G1001" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1001" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1001" s="32">
         <v>1.0</v>
       </c>
       <c r="J1001" s="5">
         <f>VLOOKUP(G1001,rewardsModel,IFS(H1001=1,2,H1001=2,3,H1001=3,4),false)*I1001</f>
         <v>0.03</v>
       </c>
+      <c r="L1001" s="3" t="s">
+        <v>1126</v>
+      </c>
     </row>
     <row r="1002">
-      <c r="A1002" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1002" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1002" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1002" s="5" t="s">
+      <c r="A1002" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1002" s="38">
+        <v>45389.0</v>
+      </c>
+      <c r="C1002" s="38">
+        <v>45415.0</v>
+      </c>
+      <c r="D1002" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1002" s="54" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G1002" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1002" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1002" s="5">
+      <c r="F1002" s="10" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G1002" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1002" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I1002" s="32">
         <v>1.0</v>
       </c>
       <c r="J1002" s="5">
         <f>VLOOKUP(G1002,rewardsModel,IFS(H1002=1,2,H1002=2,3,H1002=3,4),false)*I1002</f>
-        <v>0.03</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="1003">
-      <c r="A1003" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1003" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1003" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1003" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1003" s="54" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G1003" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1003" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1003" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1003" s="5">
-        <f>VLOOKUP(G1003,rewardsModel,IFS(H1003=1,2,H1003=2,3,H1003=3,4),false)*I1003</f>
-        <v>0.03</v>
-      </c>
+      <c r="G1003" s="5"/>
     </row>
     <row r="1004">
-      <c r="A1004" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1004" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1004" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1004" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1004" s="54" t="s">
-        <v>1123</v>
-      </c>
-      <c r="G1004" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1004" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1004" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1004" s="5">
-        <f>VLOOKUP(G1004,rewardsModel,IFS(H1004=1,2,H1004=2,3,H1004=3,4),false)*I1004</f>
-        <v>0.03</v>
-      </c>
+      <c r="A1004" s="28" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B1004" s="27"/>
+      <c r="C1004" s="28"/>
+      <c r="D1004" s="29"/>
+      <c r="E1004" s="29"/>
+      <c r="F1004" s="29"/>
+      <c r="G1004" s="29"/>
+      <c r="H1004" s="29"/>
+      <c r="I1004" s="29"/>
+      <c r="J1004" s="29"/>
+      <c r="K1004" s="29"/>
+      <c r="L1004" s="27"/>
+      <c r="M1004" s="27"/>
+      <c r="N1004" s="27"/>
+      <c r="O1004" s="27"/>
+      <c r="P1004" s="27"/>
+      <c r="Q1004" s="27"/>
+      <c r="R1004" s="27"/>
+      <c r="S1004" s="27"/>
+      <c r="T1004" s="27"/>
+      <c r="U1004" s="27"/>
+      <c r="V1004" s="27"/>
+      <c r="W1004" s="27"/>
+      <c r="X1004" s="27"/>
+      <c r="Y1004" s="27"/>
+      <c r="Z1004" s="27"/>
+      <c r="AA1004" s="27"/>
+      <c r="AB1004" s="27"/>
+      <c r="AC1004" s="27"/>
     </row>
     <row r="1005">
-      <c r="A1005" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1005" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1005" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1005" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1005" s="54" t="s">
-        <v>1123</v>
-      </c>
-      <c r="G1005" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1005" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1005" s="5">
+      <c r="A1005" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B1005" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1005" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1005" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1005" s="10" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G1005" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1005" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1005" s="32">
         <v>1.0</v>
       </c>
       <c r="J1005" s="5">
@@ -50563,28 +50708,28 @@
       </c>
     </row>
     <row r="1006">
-      <c r="A1006" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1006" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1006" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1006" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1006" s="54" t="s">
-        <v>1124</v>
-      </c>
-      <c r="G1006" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1006" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1006" s="5">
+      <c r="A1006" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1006" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1006" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1006" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1006" s="10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G1006" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1006" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1006" s="32">
         <v>1.0</v>
       </c>
       <c r="J1006" s="5">
@@ -50593,28 +50738,28 @@
       </c>
     </row>
     <row r="1007">
-      <c r="A1007" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="B1007" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1007" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1007" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1007" s="54" t="s">
-        <v>1124</v>
-      </c>
-      <c r="G1007" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1007" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1007" s="5">
+      <c r="A1007" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B1007" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1007" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1007" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1007" s="10" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G1007" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1007" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1007" s="32">
         <v>1.0</v>
       </c>
       <c r="J1007" s="5">
@@ -50623,28 +50768,28 @@
       </c>
     </row>
     <row r="1008">
-      <c r="A1008" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1008" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1008" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1008" s="5" t="s">
+      <c r="A1008" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1008" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1008" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1008" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1008" s="54" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G1008" s="5" t="s">
+      <c r="F1008" s="10" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G1008" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="H1008" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1008" s="5">
+      <c r="H1008" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1008" s="32">
         <v>1.0</v>
       </c>
       <c r="J1008" s="5">
@@ -50653,28 +50798,28 @@
       </c>
     </row>
     <row r="1009">
-      <c r="A1009" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1009" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1009" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1009" s="5" t="s">
+      <c r="A1009" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1009" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1009" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1009" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1009" s="54" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G1009" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1009" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1009" s="5">
+      <c r="F1009" s="10" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G1009" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1009" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1009" s="32">
         <v>1.0</v>
       </c>
       <c r="J1009" s="5">
@@ -50683,178 +50828,187 @@
       </c>
     </row>
     <row r="1010">
-      <c r="A1010" s="5" t="s">
+      <c r="A1010" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B1010" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1010" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1010" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1010" s="54" t="s">
-        <v>1125</v>
-      </c>
-      <c r="G1010" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1010" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1010" s="5">
+      <c r="B1010" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1010" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1010" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1010" s="10" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G1010" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1010" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I1010" s="32">
         <v>1.0</v>
       </c>
       <c r="J1010" s="5">
         <f>VLOOKUP(G1010,rewardsModel,IFS(H1010=1,2,H1010=2,3,H1010=3,4),false)*I1010</f>
-        <v>0.1</v>
+        <v>0.135</v>
+      </c>
+      <c r="L1010" s="3" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="1011">
-      <c r="A1011" s="5" t="s">
+      <c r="A1011" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B1011" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1011" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1011" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1011" s="54" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G1011" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1011" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1011" s="5">
+      <c r="B1011" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1011" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1011" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1011" s="10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G1011" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1011" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I1011" s="32">
         <v>1.0</v>
       </c>
       <c r="J1011" s="5">
         <f>VLOOKUP(G1011,rewardsModel,IFS(H1011=1,2,H1011=2,3,H1011=3,4),false)*I1011</f>
-        <v>0.03</v>
+        <v>0.06</v>
+      </c>
+      <c r="L1011" s="3" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="1012">
-      <c r="A1012" s="5" t="s">
+      <c r="A1012" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B1012" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1012" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1012" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1012" s="54" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G1012" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1012" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1012" s="5">
+      <c r="B1012" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1012" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1012" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1012" s="10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G1012" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1012" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1012" s="32">
         <v>1.0</v>
       </c>
       <c r="J1012" s="5">
         <f>VLOOKUP(G1012,rewardsModel,IFS(H1012=1,2,H1012=2,3,H1012=3,4),false)*I1012</f>
         <v>0.03</v>
       </c>
+      <c r="L1012" s="3" t="s">
+        <v>1142</v>
+      </c>
     </row>
     <row r="1013">
-      <c r="A1013" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1013" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1013" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1013" s="5" t="s">
+      <c r="A1013" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1013" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1013" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1013" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1013" s="54" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G1013" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1013" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1013" s="5">
+      <c r="F1013" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G1013" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1013" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I1013" s="32">
         <v>1.0</v>
       </c>
       <c r="J1013" s="5">
         <f>VLOOKUP(G1013,rewardsModel,IFS(H1013=1,2,H1013=2,3,H1013=3,4),false)*I1013</f>
-        <v>0.1</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="1014">
-      <c r="A1014" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1014" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1014" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1014" s="5" t="s">
+      <c r="A1014" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B1014" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1014" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1014" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1014" s="54" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G1014" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1014" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1014" s="5">
+      <c r="F1014" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G1014" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1014" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I1014" s="32">
         <v>1.0</v>
       </c>
       <c r="J1014" s="5">
         <f>VLOOKUP(G1014,rewardsModel,IFS(H1014=1,2,H1014=2,3,H1014=3,4),false)*I1014</f>
-        <v>0.03</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="1015">
-      <c r="A1015" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1015" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1015" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1015" s="5" t="s">
+      <c r="A1015" s="3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1015" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1015" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1015" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1015" s="54" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G1015" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1015" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1015" s="5">
+      <c r="F1015" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G1015" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1015" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1015" s="32">
         <v>1.0</v>
       </c>
       <c r="J1015" s="5">
@@ -50863,248 +51017,116 @@
       </c>
     </row>
     <row r="1016">
-      <c r="A1016" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1016" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1016" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1016" s="5" t="s">
+      <c r="A1016" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1016" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1016" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1016" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1016" s="54" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G1016" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1016" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1016" s="5">
+      <c r="F1016" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G1016" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1016" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I1016" s="32">
         <v>1.0</v>
       </c>
       <c r="J1016" s="5">
         <f>VLOOKUP(G1016,rewardsModel,IFS(H1016=1,2,H1016=2,3,H1016=3,4),false)*I1016</f>
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1017">
-      <c r="A1017" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1017" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1017" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1017" s="5" t="s">
+      <c r="A1017" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1017" s="38">
+        <v>45416.0</v>
+      </c>
+      <c r="C1017" s="38">
+        <v>45443.0</v>
+      </c>
+      <c r="D1017" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="F1017" s="54" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G1017" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1017" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1017" s="5">
+      <c r="F1017" s="10" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G1017" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1017" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I1017" s="32">
         <v>1.0</v>
       </c>
       <c r="J1017" s="5">
         <f>VLOOKUP(G1017,rewardsModel,IFS(H1017=1,2,H1017=2,3,H1017=3,4),false)*I1017</f>
-        <v>0.03</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="1018">
-      <c r="A1018" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1018" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1018" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1018" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1018" s="54" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G1018" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1018" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1018" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1018" s="5">
-        <f>VLOOKUP(G1018,rewardsModel,IFS(H1018=1,2,H1018=2,3,H1018=3,4),false)*I1018</f>
-        <v>0.03</v>
-      </c>
+      <c r="G1018" s="45"/>
     </row>
     <row r="1019">
-      <c r="A1019" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1019" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1019" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1019" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1019" s="54" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G1019" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1019" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="I1019" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1019" s="5">
-        <f>VLOOKUP(G1019,rewardsModel,IFS(H1019=1,2,H1019=2,3,H1019=3,4),false)*I1019</f>
-        <v>0.2</v>
-      </c>
+      <c r="G1019" s="45"/>
     </row>
     <row r="1020">
-      <c r="A1020" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1020" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1020" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1020" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1020" s="54" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G1020" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1020" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1020" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1020" s="5">
-        <f>VLOOKUP(G1020,rewardsModel,IFS(H1020=1,2,H1020=2,3,H1020=3,4),false)*I1020</f>
-        <v>0.03</v>
-      </c>
+      <c r="G1020" s="45"/>
     </row>
     <row r="1021">
-      <c r="A1021" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1021" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1021" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1021" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1021" s="54" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G1021" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1021" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1021" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1021" s="5">
-        <f>VLOOKUP(G1021,rewardsModel,IFS(H1021=1,2,H1021=2,3,H1021=3,4),false)*I1021</f>
-        <v>0.03</v>
-      </c>
+      <c r="G1021" s="45"/>
     </row>
     <row r="1022">
-      <c r="A1022" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1022" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1022" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1022" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1022" s="54" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G1022" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1022" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="I1022" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1022" s="5">
-        <f>VLOOKUP(G1022,rewardsModel,IFS(H1022=1,2,H1022=2,3,H1022=3,4),false)*I1022</f>
-        <v>0.2</v>
-      </c>
+      <c r="G1022" s="45"/>
     </row>
     <row r="1023">
-      <c r="A1023" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1023" s="5">
-        <v>45276.0</v>
-      </c>
-      <c r="C1023" s="5">
-        <v>45303.0</v>
-      </c>
-      <c r="D1023" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1023" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="G1023" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1023" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I1023" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J1023" s="5">
-        <f>VLOOKUP(G1023,rewardsModel,IFS(H1023=1,2,H1023=2,3,H1023=3,4),false)*I1023</f>
-        <v>0.03</v>
-      </c>
+      <c r="A1023" s="28" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1023" s="27"/>
+      <c r="C1023" s="28"/>
+      <c r="D1023" s="29"/>
+      <c r="E1023" s="29"/>
+      <c r="F1023" s="29"/>
+      <c r="G1023" s="29"/>
+      <c r="H1023" s="29"/>
+      <c r="I1023" s="29"/>
+      <c r="J1023" s="29"/>
+      <c r="K1023" s="29"/>
+      <c r="L1023" s="27"/>
+      <c r="M1023" s="27"/>
+      <c r="N1023" s="27"/>
+      <c r="O1023" s="27"/>
+      <c r="P1023" s="27"/>
+      <c r="Q1023" s="27"/>
+      <c r="R1023" s="27"/>
+      <c r="S1023" s="27"/>
+      <c r="T1023" s="27"/>
+      <c r="U1023" s="27"/>
+      <c r="V1023" s="27"/>
+      <c r="W1023" s="27"/>
+      <c r="X1023" s="27"/>
+      <c r="Y1023" s="27"/>
+      <c r="Z1023" s="27"/>
+      <c r="AA1023" s="27"/>
+      <c r="AB1023" s="27"/>
+      <c r="AC1023" s="27"/>
     </row>
     <row r="1024">
       <c r="A1024" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1024" s="5">
         <v>45276.0</v>
@@ -51116,10 +51138,10 @@
         <v>477</v>
       </c>
       <c r="F1024" s="54" t="s">
-        <v>1130</v>
+        <v>1148</v>
       </c>
       <c r="G1024" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1024" s="5">
         <v>1.0</v>
@@ -51134,7 +51156,7 @@
     </row>
     <row r="1025">
       <c r="A1025" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1025" s="5">
         <v>45276.0</v>
@@ -51146,12 +51168,12 @@
         <v>477</v>
       </c>
       <c r="F1025" s="54" t="s">
-        <v>1131</v>
+        <v>1148</v>
       </c>
       <c r="G1025" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1025" s="5">
+        <v>91</v>
+      </c>
+      <c r="H1025" s="3">
         <v>1.0</v>
       </c>
       <c r="I1025" s="5">
@@ -51164,7 +51186,7 @@
     </row>
     <row r="1026">
       <c r="A1026" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1026" s="5">
         <v>45276.0</v>
@@ -51176,10 +51198,10 @@
         <v>477</v>
       </c>
       <c r="F1026" s="54" t="s">
-        <v>1131</v>
+        <v>1149</v>
       </c>
       <c r="G1026" s="5" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="H1026" s="5">
         <v>1.0</v>
@@ -51194,7 +51216,7 @@
     </row>
     <row r="1027">
       <c r="A1027" s="5" t="s">
-        <v>980</v>
+        <v>652</v>
       </c>
       <c r="B1027" s="5">
         <v>45276.0</v>
@@ -51203,10 +51225,10 @@
         <v>45303.0</v>
       </c>
       <c r="D1027" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1027" s="54" t="s">
-        <v>1132</v>
+        <v>1149</v>
       </c>
       <c r="G1027" s="5" t="s">
         <v>91</v>
@@ -51224,7 +51246,7 @@
     </row>
     <row r="1028">
       <c r="A1028" s="5" t="s">
-        <v>980</v>
+        <v>652</v>
       </c>
       <c r="B1028" s="5">
         <v>45276.0</v>
@@ -51233,13 +51255,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1028" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1028" s="54" t="s">
-        <v>1133</v>
+        <v>1150</v>
       </c>
       <c r="G1028" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1028" s="5">
         <v>1.0</v>
@@ -51254,7 +51276,7 @@
     </row>
     <row r="1029">
       <c r="A1029" s="5" t="s">
-        <v>980</v>
+        <v>652</v>
       </c>
       <c r="B1029" s="5">
         <v>45276.0</v>
@@ -51263,10 +51285,10 @@
         <v>45303.0</v>
       </c>
       <c r="D1029" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1029" s="54" t="s">
-        <v>1134</v>
+        <v>1150</v>
       </c>
       <c r="G1029" s="5" t="s">
         <v>91</v>
@@ -51284,7 +51306,7 @@
     </row>
     <row r="1030">
       <c r="A1030" s="5" t="s">
-        <v>852</v>
+        <v>652</v>
       </c>
       <c r="B1030" s="5">
         <v>45276.0</v>
@@ -51293,28 +51315,28 @@
         <v>45303.0</v>
       </c>
       <c r="D1030" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1030" s="54" t="s">
-        <v>1135</v>
+        <v>1151</v>
       </c>
       <c r="G1030" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1030" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1030" s="5">
         <v>1.0</v>
       </c>
       <c r="J1030" s="5">
         <f>VLOOKUP(G1030,rewardsModel,IFS(H1030=1,2,H1030=2,3,H1030=3,4),false)*I1030</f>
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1031">
       <c r="A1031" s="5" t="s">
-        <v>852</v>
+        <v>652</v>
       </c>
       <c r="B1031" s="5">
         <v>45276.0</v>
@@ -51323,10 +51345,10 @@
         <v>45303.0</v>
       </c>
       <c r="D1031" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1031" s="54" t="s">
-        <v>1136</v>
+        <v>1151</v>
       </c>
       <c r="G1031" s="5" t="s">
         <v>91</v>
@@ -51344,7 +51366,7 @@
     </row>
     <row r="1032">
       <c r="A1032" s="5" t="s">
-        <v>348</v>
+        <v>652</v>
       </c>
       <c r="B1032" s="5">
         <v>45276.0</v>
@@ -51353,13 +51375,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1032" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1032" s="54" t="s">
-        <v>1137</v>
+        <v>1152</v>
       </c>
       <c r="G1032" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1032" s="5">
         <v>1.0</v>
@@ -51374,7 +51396,7 @@
     </row>
     <row r="1033">
       <c r="A1033" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1033" s="5">
         <v>45276.0</v>
@@ -51386,10 +51408,10 @@
         <v>477</v>
       </c>
       <c r="F1033" s="54" t="s">
-        <v>1138</v>
+        <v>1152</v>
       </c>
       <c r="G1033" s="5" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="H1033" s="5">
         <v>1.0</v>
@@ -51399,12 +51421,12 @@
       </c>
       <c r="J1033" s="5">
         <f>VLOOKUP(G1033,rewardsModel,IFS(H1033=1,2,H1033=2,3,H1033=3,4),false)*I1033</f>
-        <v>0.035</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1034">
       <c r="A1034" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1034" s="5">
         <v>45276.0</v>
@@ -51416,25 +51438,25 @@
         <v>477</v>
       </c>
       <c r="F1034" s="54" t="s">
-        <v>1139</v>
+        <v>1153</v>
       </c>
       <c r="G1034" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1034" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1034" s="5">
         <v>1.0</v>
       </c>
       <c r="J1034" s="5">
         <f>VLOOKUP(G1034,rewardsModel,IFS(H1034=1,2,H1034=2,3,H1034=3,4),false)*I1034</f>
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1035">
       <c r="A1035" s="5" t="s">
-        <v>1140</v>
+        <v>652</v>
       </c>
       <c r="B1035" s="5">
         <v>45276.0</v>
@@ -51443,28 +51465,28 @@
         <v>45303.0</v>
       </c>
       <c r="D1035" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1035" s="54" t="s">
-        <v>1141</v>
+        <v>1153</v>
       </c>
       <c r="G1035" s="5" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="H1035" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1035" s="5">
         <v>1.0</v>
       </c>
       <c r="J1035" s="5">
         <f>VLOOKUP(G1035,rewardsModel,IFS(H1035=1,2,H1035=2,3,H1035=3,4),false)*I1035</f>
-        <v>0.07</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1036">
       <c r="A1036" s="5" t="s">
-        <v>348</v>
+        <v>652</v>
       </c>
       <c r="B1036" s="5">
         <v>45276.0</v>
@@ -51473,13 +51495,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1036" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1036" s="54" t="s">
-        <v>1141</v>
+        <v>1154</v>
       </c>
       <c r="G1036" s="5" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="H1036" s="5">
         <v>1.0</v>
@@ -51489,12 +51511,12 @@
       </c>
       <c r="J1036" s="5">
         <f>VLOOKUP(G1036,rewardsModel,IFS(H1036=1,2,H1036=2,3,H1036=3,4),false)*I1036</f>
-        <v>0.035</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1037">
       <c r="A1037" s="5" t="s">
-        <v>1088</v>
+        <v>652</v>
       </c>
       <c r="B1037" s="5">
         <v>45276.0</v>
@@ -51506,25 +51528,25 @@
         <v>477</v>
       </c>
       <c r="F1037" s="54" t="s">
-        <v>1142</v>
+        <v>1154</v>
       </c>
       <c r="G1037" s="5" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="H1037" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1037" s="5">
         <v>1.0</v>
       </c>
       <c r="J1037" s="5">
         <f>VLOOKUP(G1037,rewardsModel,IFS(H1037=1,2,H1037=2,3,H1037=3,4),false)*I1037</f>
-        <v>0.135</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1038">
       <c r="A1038" s="5" t="s">
-        <v>1143</v>
+        <v>652</v>
       </c>
       <c r="B1038" s="5">
         <v>45276.0</v>
@@ -51533,13 +51555,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1038" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1038" s="54" t="s">
-        <v>1144</v>
+        <v>1155</v>
       </c>
       <c r="G1038" s="5" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="H1038" s="5">
         <v>1.0</v>
@@ -51554,7 +51576,7 @@
     </row>
     <row r="1039">
       <c r="A1039" s="5" t="s">
-        <v>1145</v>
+        <v>652</v>
       </c>
       <c r="B1039" s="5">
         <v>45276.0</v>
@@ -51563,13 +51585,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1039" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1039" s="54" t="s">
-        <v>1142</v>
+        <v>1155</v>
       </c>
       <c r="G1039" s="5" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="H1039" s="5">
         <v>1.0</v>
@@ -51584,7 +51606,7 @@
     </row>
     <row r="1040">
       <c r="A1040" s="5" t="s">
-        <v>426</v>
+        <v>652</v>
       </c>
       <c r="B1040" s="5">
         <v>45276.0</v>
@@ -51593,13 +51615,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1040" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1040" s="54" t="s">
-        <v>1142</v>
+        <v>1156</v>
       </c>
       <c r="G1040" s="5" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="H1040" s="5">
         <v>1.0</v>
@@ -51614,7 +51636,7 @@
     </row>
     <row r="1041">
       <c r="A1041" s="5" t="s">
-        <v>980</v>
+        <v>652</v>
       </c>
       <c r="B1041" s="5">
         <v>45276.0</v>
@@ -51623,13 +51645,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1041" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1041" s="54" t="s">
-        <v>1146</v>
+        <v>1156</v>
       </c>
       <c r="G1041" s="5" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="H1041" s="5">
         <v>1.0</v>
@@ -51644,7 +51666,7 @@
     </row>
     <row r="1042">
       <c r="A1042" s="5" t="s">
-        <v>348</v>
+        <v>426</v>
       </c>
       <c r="B1042" s="5">
         <v>45276.0</v>
@@ -51656,20 +51678,20 @@
         <v>477</v>
       </c>
       <c r="F1042" s="54" t="s">
-        <v>1147</v>
+        <v>1157</v>
       </c>
       <c r="G1042" s="5" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="H1042" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1042" s="5">
         <v>1.0</v>
       </c>
       <c r="J1042" s="5">
         <f>VLOOKUP(G1042,rewardsModel,IFS(H1042=1,2,H1042=2,3,H1042=3,4),false)*I1042</f>
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1043">
@@ -51686,10 +51708,10 @@
         <v>477</v>
       </c>
       <c r="F1043" s="54" t="s">
-        <v>1148</v>
+        <v>1157</v>
       </c>
       <c r="G1043" s="5" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="H1043" s="5">
         <v>1.0</v>
@@ -51716,10 +51738,10 @@
         <v>477</v>
       </c>
       <c r="F1044" s="54" t="s">
-        <v>1148</v>
+        <v>1157</v>
       </c>
       <c r="G1044" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H1044" s="5">
         <v>1.0</v>
@@ -51729,12 +51751,12 @@
       </c>
       <c r="J1044" s="5">
         <f>VLOOKUP(G1044,rewardsModel,IFS(H1044=1,2,H1044=2,3,H1044=3,4),false)*I1044</f>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="1045">
       <c r="A1045" s="5" t="s">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="B1045" s="5">
         <v>45276.0</v>
@@ -51743,13 +51765,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1045" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1045" s="54" t="s">
-        <v>1149</v>
+        <v>1158</v>
       </c>
       <c r="G1045" s="5" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="H1045" s="5">
         <v>1.0</v>
@@ -51773,23 +51795,23 @@
         <v>45303.0</v>
       </c>
       <c r="D1046" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1046" s="54" t="s">
-        <v>1150</v>
+        <v>1158</v>
       </c>
       <c r="G1046" s="5" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="H1046" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1046" s="5">
         <v>1.0</v>
       </c>
       <c r="J1046" s="5">
         <f>VLOOKUP(G1046,rewardsModel,IFS(H1046=1,2,H1046=2,3,H1046=3,4),false)*I1046</f>
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1047">
@@ -51803,13 +51825,13 @@
         <v>45303.0</v>
       </c>
       <c r="D1047" s="5" t="s">
-        <v>193</v>
+        <v>477</v>
       </c>
       <c r="F1047" s="54" t="s">
-        <v>1151</v>
+        <v>1158</v>
       </c>
       <c r="G1047" s="5" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="H1047" s="5">
         <v>1.0</v>
@@ -51819,12 +51841,12 @@
       </c>
       <c r="J1047" s="5">
         <f>VLOOKUP(G1047,rewardsModel,IFS(H1047=1,2,H1047=2,3,H1047=3,4),false)*I1047</f>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="1048">
       <c r="A1048" s="5" t="s">
-        <v>369</v>
+        <v>426</v>
       </c>
       <c r="B1048" s="5">
         <v>45276.0</v>
@@ -51836,20 +51858,20 @@
         <v>477</v>
       </c>
       <c r="F1048" s="54" t="s">
-        <v>1152</v>
+        <v>1159</v>
       </c>
       <c r="G1048" s="5" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="H1048" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1048" s="5">
         <v>1.0</v>
       </c>
       <c r="J1048" s="5">
         <f>VLOOKUP(G1048,rewardsModel,IFS(H1048=1,2,H1048=2,3,H1048=3,4),false)*I1048</f>
-        <v>0.07</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1049">
@@ -51866,10 +51888,10 @@
         <v>477</v>
       </c>
       <c r="F1049" s="54" t="s">
-        <v>1153</v>
+        <v>1159</v>
       </c>
       <c r="G1049" s="5" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="H1049" s="5">
         <v>1.0</v>
@@ -51896,10 +51918,10 @@
         <v>477</v>
       </c>
       <c r="F1050" s="54" t="s">
-        <v>1153</v>
+        <v>1159</v>
       </c>
       <c r="G1050" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H1050" s="5">
         <v>1.0</v>
@@ -51909,12 +51931,12 @@
       </c>
       <c r="J1050" s="5">
         <f>VLOOKUP(G1050,rewardsModel,IFS(H1050=1,2,H1050=2,3,H1050=3,4),false)*I1050</f>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="1051">
       <c r="A1051" s="5" t="s">
-        <v>327</v>
+        <v>426</v>
       </c>
       <c r="B1051" s="5">
         <v>45276.0</v>
@@ -51926,7 +51948,7 @@
         <v>477</v>
       </c>
       <c r="F1051" s="54" t="s">
-        <v>1154</v>
+        <v>1160</v>
       </c>
       <c r="G1051" s="5" t="s">
         <v>97</v>
@@ -51944,7 +51966,7 @@
     </row>
     <row r="1052">
       <c r="A1052" s="5" t="s">
-        <v>327</v>
+        <v>426</v>
       </c>
       <c r="B1052" s="5">
         <v>45276.0</v>
@@ -51956,7 +51978,7 @@
         <v>477</v>
       </c>
       <c r="F1052" s="54" t="s">
-        <v>1154</v>
+        <v>1160</v>
       </c>
       <c r="G1052" s="5" t="s">
         <v>56</v>
@@ -51974,7 +51996,7 @@
     </row>
     <row r="1053">
       <c r="A1053" s="5" t="s">
-        <v>652</v>
+        <v>426</v>
       </c>
       <c r="B1053" s="5">
         <v>45276.0</v>
@@ -51986,10 +52008,10 @@
         <v>477</v>
       </c>
       <c r="F1053" s="54" t="s">
-        <v>1155</v>
+        <v>1160</v>
       </c>
       <c r="G1053" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H1053" s="5">
         <v>2.0</v>
@@ -51999,12 +52021,12 @@
       </c>
       <c r="J1053" s="5">
         <f>VLOOKUP(G1053,rewardsModel,IFS(H1053=1,2,H1053=2,3,H1053=3,4),false)*I1053</f>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="1054">
       <c r="A1054" s="5" t="s">
-        <v>327</v>
+        <v>426</v>
       </c>
       <c r="B1054" s="5">
         <v>45276.0</v>
@@ -52016,25 +52038,25 @@
         <v>477</v>
       </c>
       <c r="F1054" s="54" t="s">
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c r="G1054" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1054" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I1054" s="5">
         <v>1.0</v>
       </c>
       <c r="J1054" s="5">
         <f>VLOOKUP(G1054,rewardsModel,IFS(H1054=1,2,H1054=2,3,H1054=3,4),false)*I1054</f>
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="1055">
       <c r="A1055" s="5" t="s">
-        <v>852</v>
+        <v>426</v>
       </c>
       <c r="B1055" s="5">
         <v>45276.0</v>
@@ -52046,10 +52068,10 @@
         <v>477</v>
       </c>
       <c r="F1055" s="54" t="s">
-        <v>1156</v>
+        <v>1161</v>
       </c>
       <c r="G1055" s="5" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="H1055" s="5">
         <v>1.0</v>
@@ -52076,123 +52098,1041 @@
         <v>477</v>
       </c>
       <c r="F1056" s="54" t="s">
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c r="G1056" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="H1056" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I1056" s="5">
         <v>1.0</v>
       </c>
       <c r="J1056" s="5">
         <f>VLOOKUP(G1056,rewardsModel,IFS(H1056=1,2,H1056=2,3,H1056=3,4),false)*I1056</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1057" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1057" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1057" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1057" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G1057" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1057" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1057" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1057" s="5">
+        <f>VLOOKUP(G1057,rewardsModel,IFS(H1057=1,2,H1057=2,3,H1057=3,4),false)*I1057</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="1057">
-      <c r="G1057" s="5"/>
-    </row>
     <row r="1058">
-      <c r="G1058" s="5"/>
+      <c r="A1058" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1058" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1058" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1058" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1058" s="54" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G1058" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1058" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1058" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1058" s="5">
+        <f>VLOOKUP(G1058,rewardsModel,IFS(H1058=1,2,H1058=2,3,H1058=3,4),false)*I1058</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1059">
-      <c r="G1059" s="5"/>
+      <c r="A1059" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1059" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1059" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1059" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1059" s="54" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G1059" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1059" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1059" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1059" s="5">
+        <f>VLOOKUP(G1059,rewardsModel,IFS(H1059=1,2,H1059=2,3,H1059=3,4),false)*I1059</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1060">
-      <c r="G1060" s="5"/>
+      <c r="A1060" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1060" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1060" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1060" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1060" s="54" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G1060" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1060" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1060" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1060" s="5">
+        <f>VLOOKUP(G1060,rewardsModel,IFS(H1060=1,2,H1060=2,3,H1060=3,4),false)*I1060</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1061">
-      <c r="G1061" s="5"/>
+      <c r="A1061" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1061" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1061" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1061" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1061" s="54" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G1061" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1061" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1061" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1061" s="5">
+        <f>VLOOKUP(G1061,rewardsModel,IFS(H1061=1,2,H1061=2,3,H1061=3,4),false)*I1061</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1062">
-      <c r="G1062" s="5"/>
+      <c r="A1062" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1062" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1062" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1062" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1062" s="54" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G1062" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1062" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1062" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1062" s="5">
+        <f>VLOOKUP(G1062,rewardsModel,IFS(H1062=1,2,H1062=2,3,H1062=3,4),false)*I1062</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1063">
-      <c r="G1063" s="5"/>
+      <c r="A1063" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1063" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1063" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1063" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1063" s="54" t="s">
+        <v>1166</v>
+      </c>
+      <c r="G1063" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1063" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1063" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1063" s="5">
+        <f>VLOOKUP(G1063,rewardsModel,IFS(H1063=1,2,H1063=2,3,H1063=3,4),false)*I1063</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1064">
-      <c r="G1064" s="5"/>
+      <c r="A1064" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B1064" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1064" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1064" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1064" s="54" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G1064" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1064" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1064" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1064" s="5">
+        <f>VLOOKUP(G1064,rewardsModel,IFS(H1064=1,2,H1064=2,3,H1064=3,4),false)*I1064</f>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="1065">
-      <c r="G1065" s="5"/>
+      <c r="A1065" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B1065" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1065" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1065" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1065" s="54" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1065" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1065" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1065" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1065" s="5">
+        <f>VLOOKUP(G1065,rewardsModel,IFS(H1065=1,2,H1065=2,3,H1065=3,4),false)*I1065</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1066">
-      <c r="G1066" s="5"/>
+      <c r="A1066" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1066" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1066" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1066" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1066" s="54" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G1066" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1066" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1066" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1066" s="5">
+        <f>VLOOKUP(G1066,rewardsModel,IFS(H1066=1,2,H1066=2,3,H1066=3,4),false)*I1066</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1067">
-      <c r="G1067" s="5"/>
+      <c r="A1067" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1067" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1067" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1067" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1067" s="54" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G1067" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1067" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1067" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1067" s="5">
+        <f>VLOOKUP(G1067,rewardsModel,IFS(H1067=1,2,H1067=2,3,H1067=3,4),false)*I1067</f>
+        <v>0.035</v>
+      </c>
     </row>
     <row r="1068">
-      <c r="G1068" s="5"/>
+      <c r="A1068" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1068" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1068" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1068" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1068" s="54" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G1068" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1068" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1068" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1068" s="5">
+        <f>VLOOKUP(G1068,rewardsModel,IFS(H1068=1,2,H1068=2,3,H1068=3,4),false)*I1068</f>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="1069">
-      <c r="G1069" s="5"/>
+      <c r="A1069" s="5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B1069" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1069" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1069" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1069" s="54" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G1069" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1069" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1069" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1069" s="5">
+        <f>VLOOKUP(G1069,rewardsModel,IFS(H1069=1,2,H1069=2,3,H1069=3,4),false)*I1069</f>
+        <v>0.07</v>
+      </c>
     </row>
     <row r="1070">
-      <c r="G1070" s="5"/>
+      <c r="A1070" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1070" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1070" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1070" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1070" s="54" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G1070" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1070" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1070" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1070" s="5">
+        <f>VLOOKUP(G1070,rewardsModel,IFS(H1070=1,2,H1070=2,3,H1070=3,4),false)*I1070</f>
+        <v>0.035</v>
+      </c>
     </row>
     <row r="1071">
-      <c r="G1071" s="5"/>
+      <c r="A1071" s="5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B1071" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1071" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1071" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1071" s="54" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G1071" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1071" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="I1071" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1071" s="5">
+        <f>VLOOKUP(G1071,rewardsModel,IFS(H1071=1,2,H1071=2,3,H1071=3,4),false)*I1071</f>
+        <v>0.135</v>
+      </c>
     </row>
     <row r="1072">
-      <c r="G1072" s="5"/>
+      <c r="A1072" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B1072" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1072" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1072" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1072" s="54" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G1072" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1072" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1072" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1072" s="5">
+        <f>VLOOKUP(G1072,rewardsModel,IFS(H1072=1,2,H1072=2,3,H1072=3,4),false)*I1072</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1073">
-      <c r="G1073" s="5"/>
+      <c r="A1073" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B1073" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1073" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1073" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1073" s="54" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G1073" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1073" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1073" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1073" s="5">
+        <f>VLOOKUP(G1073,rewardsModel,IFS(H1073=1,2,H1073=2,3,H1073=3,4),false)*I1073</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1074">
-      <c r="G1074" s="5"/>
+      <c r="A1074" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1074" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1074" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1074" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1074" s="54" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G1074" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1074" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1074" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1074" s="5">
+        <f>VLOOKUP(G1074,rewardsModel,IFS(H1074=1,2,H1074=2,3,H1074=3,4),false)*I1074</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1075">
-      <c r="G1075" s="5"/>
+      <c r="A1075" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1075" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1075" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1075" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1075" s="54" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G1075" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1075" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1075" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1075" s="5">
+        <f>VLOOKUP(G1075,rewardsModel,IFS(H1075=1,2,H1075=2,3,H1075=3,4),false)*I1075</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1076">
-      <c r="G1076" s="5"/>
+      <c r="A1076" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1076" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1076" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1076" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1076" s="54" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1076" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1076" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="I1076" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1076" s="5">
+        <f>VLOOKUP(G1076,rewardsModel,IFS(H1076=1,2,H1076=2,3,H1076=3,4),false)*I1076</f>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="1077">
-      <c r="G1077" s="5"/>
+      <c r="A1077" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1077" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1077" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1077" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1077" s="54" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G1077" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1077" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1077" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1077" s="5">
+        <f>VLOOKUP(G1077,rewardsModel,IFS(H1077=1,2,H1077=2,3,H1077=3,4),false)*I1077</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1078">
-      <c r="G1078" s="5"/>
+      <c r="A1078" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1078" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1078" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1078" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1078" s="54" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G1078" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1078" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1078" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1078" s="5">
+        <f>VLOOKUP(G1078,rewardsModel,IFS(H1078=1,2,H1078=2,3,H1078=3,4),false)*I1078</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1079">
-      <c r="G1079" s="5"/>
+      <c r="A1079" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1079" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1079" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1079" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1079" s="54" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G1079" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1079" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1079" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1079" s="5">
+        <f>VLOOKUP(G1079,rewardsModel,IFS(H1079=1,2,H1079=2,3,H1079=3,4),false)*I1079</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1080">
-      <c r="G1080" s="5"/>
+      <c r="A1080" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1080" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1080" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1080" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1080" s="54" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G1080" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1080" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1080" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1080" s="5">
+        <f>VLOOKUP(G1080,rewardsModel,IFS(H1080=1,2,H1080=2,3,H1080=3,4),false)*I1080</f>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="1081">
-      <c r="G1081" s="5"/>
+      <c r="A1081" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1081" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1081" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1081" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1081" s="54" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G1081" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1081" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1081" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1081" s="5">
+        <f>VLOOKUP(G1081,rewardsModel,IFS(H1081=1,2,H1081=2,3,H1081=3,4),false)*I1081</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1082">
-      <c r="G1082" s="5"/>
+      <c r="A1082" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1082" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1082" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1082" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1082" s="54" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G1082" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1082" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1082" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1082" s="5">
+        <f>VLOOKUP(G1082,rewardsModel,IFS(H1082=1,2,H1082=2,3,H1082=3,4),false)*I1082</f>
+        <v>0.07</v>
+      </c>
     </row>
     <row r="1083">
-      <c r="G1083" s="5"/>
+      <c r="A1083" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1083" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1083" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1083" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1083" s="54" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G1083" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1083" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1083" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1083" s="5">
+        <f>VLOOKUP(G1083,rewardsModel,IFS(H1083=1,2,H1083=2,3,H1083=3,4),false)*I1083</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1084">
-      <c r="G1084" s="5"/>
+      <c r="A1084" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1084" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1084" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1084" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1084" s="54" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G1084" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1084" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1084" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1084" s="5">
+        <f>VLOOKUP(G1084,rewardsModel,IFS(H1084=1,2,H1084=2,3,H1084=3,4),false)*I1084</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1085">
-      <c r="G1085" s="5"/>
+      <c r="A1085" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1085" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1085" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1085" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1085" s="54" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G1085" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1085" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1085" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1085" s="5">
+        <f>VLOOKUP(G1085,rewardsModel,IFS(H1085=1,2,H1085=2,3,H1085=3,4),false)*I1085</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1086">
-      <c r="G1086" s="5"/>
+      <c r="A1086" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1086" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1086" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1086" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1086" s="54" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G1086" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1086" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1086" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1086" s="5">
+        <f>VLOOKUP(G1086,rewardsModel,IFS(H1086=1,2,H1086=2,3,H1086=3,4),false)*I1086</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1087">
-      <c r="G1087" s="5"/>
+      <c r="A1087" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B1087" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1087" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1087" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1087" s="54" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1087" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1087" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1087" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1087" s="5">
+        <f>VLOOKUP(G1087,rewardsModel,IFS(H1087=1,2,H1087=2,3,H1087=3,4),false)*I1087</f>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="1088">
-      <c r="G1088" s="5"/>
+      <c r="A1088" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1088" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1088" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1088" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1088" s="54" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1088" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1088" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="I1088" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1088" s="5">
+        <f>VLOOKUP(G1088,rewardsModel,IFS(H1088=1,2,H1088=2,3,H1088=3,4),false)*I1088</f>
+        <v>0.06</v>
+      </c>
     </row>
     <row r="1089">
-      <c r="G1089" s="5"/>
+      <c r="A1089" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B1089" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1089" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1089" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1089" s="54" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G1089" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1089" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1089" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1089" s="5">
+        <f>VLOOKUP(G1089,rewardsModel,IFS(H1089=1,2,H1089=2,3,H1089=3,4),false)*I1089</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1090">
-      <c r="G1090" s="5"/>
+      <c r="A1090" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1090" s="5">
+        <v>45276.0</v>
+      </c>
+      <c r="C1090" s="5">
+        <v>45303.0</v>
+      </c>
+      <c r="D1090" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1090" s="54" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1090" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1090" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="I1090" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J1090" s="5">
+        <f>VLOOKUP(G1090,rewardsModel,IFS(H1090=1,2,H1090=2,3,H1090=3,4),false)*I1090</f>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="1091">
       <c r="G1091" s="5"/>
@@ -55034,17 +55974,119 @@
     </row>
     <row r="2037">
       <c r="G2037" s="5"/>
+    </row>
+    <row r="2038">
+      <c r="G2038" s="5"/>
+    </row>
+    <row r="2039">
+      <c r="G2039" s="5"/>
+    </row>
+    <row r="2040">
+      <c r="G2040" s="5"/>
+    </row>
+    <row r="2041">
+      <c r="G2041" s="5"/>
+    </row>
+    <row r="2042">
+      <c r="G2042" s="5"/>
+    </row>
+    <row r="2043">
+      <c r="G2043" s="5"/>
+    </row>
+    <row r="2044">
+      <c r="G2044" s="5"/>
+    </row>
+    <row r="2045">
+      <c r="G2045" s="5"/>
+    </row>
+    <row r="2046">
+      <c r="G2046" s="5"/>
+    </row>
+    <row r="2047">
+      <c r="G2047" s="5"/>
+    </row>
+    <row r="2048">
+      <c r="G2048" s="5"/>
+    </row>
+    <row r="2049">
+      <c r="G2049" s="5"/>
+    </row>
+    <row r="2050">
+      <c r="G2050" s="5"/>
+    </row>
+    <row r="2051">
+      <c r="G2051" s="5"/>
+    </row>
+    <row r="2052">
+      <c r="G2052" s="5"/>
+    </row>
+    <row r="2053">
+      <c r="G2053" s="5"/>
+    </row>
+    <row r="2054">
+      <c r="G2054" s="5"/>
+    </row>
+    <row r="2055">
+      <c r="G2055" s="5"/>
+    </row>
+    <row r="2056">
+      <c r="G2056" s="5"/>
+    </row>
+    <row r="2057">
+      <c r="G2057" s="5"/>
+    </row>
+    <row r="2058">
+      <c r="G2058" s="5"/>
+    </row>
+    <row r="2059">
+      <c r="G2059" s="5"/>
+    </row>
+    <row r="2060">
+      <c r="G2060" s="5"/>
+    </row>
+    <row r="2061">
+      <c r="G2061" s="5"/>
+    </row>
+    <row r="2062">
+      <c r="G2062" s="5"/>
+    </row>
+    <row r="2063">
+      <c r="G2063" s="5"/>
+    </row>
+    <row r="2064">
+      <c r="G2064" s="5"/>
+    </row>
+    <row r="2065">
+      <c r="G2065" s="5"/>
+    </row>
+    <row r="2066">
+      <c r="G2066" s="5"/>
+    </row>
+    <row r="2067">
+      <c r="G2067" s="5"/>
+    </row>
+    <row r="2068">
+      <c r="G2068" s="5"/>
+    </row>
+    <row r="2069">
+      <c r="G2069" s="5"/>
+    </row>
+    <row r="2070">
+      <c r="G2070" s="5"/>
+    </row>
+    <row r="2071">
+      <c r="G2071" s="5"/>
     </row>
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="G120:G122 G127 G129 G159:G164 G179 G183:G186 G204">
-      <formula1>'Contribution Types and Levels'!$A$5:A2037</formula1>
+      <formula1>'Contribution Types and Levels'!$A$5:A2071</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G54:G86">
-      <formula1>'Contribution Types and Levels'!$A$5:$A2037</formula1>
+      <formula1>'Contribution Types and Levels'!$A$5:$A2071</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G3:G52 G88:G119 G123:G126 G128 G130:G143 G145:G158 G165:G178 G180:G181 G187:G203 G205:G206 G208:G233 G235:G262 G264:G292 G294:G331 G333:G379 G381:G456 G458:G512 G514:G564 G566:G589 G591:G619 G621:G662 G664:G707 G709:G729 G731:G790 G792:G841 G843:G897 G899:G956 G959:G970 G972:G988 G990:G2037">
-      <formula1>'Contributions Sample (Group A)'!$D$3:$D2037</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="G3:G52 G88:G119 G123:G126 G128 G130:G143 G145:G158 G165:G178 G180:G181 G187:G203 G205:G206 G208:G233 G235:G262 G264:G292 G294:G331 G333:G379 G381:G456 G458:G512 G514:G564 G566:G589 G591:G619 G621:G662 G664:G707 G709:G729 G731:G790 G792:G841 G843:G897 G899:G956 G959:G970 G972:G988 G990:G1003 G1005:G1022 G1024:G2071">
+      <formula1>'Contributions Sample (Group A)'!$D$3:$D2071</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -56003,63 +57045,89 @@
     <hyperlink r:id="rId954" ref="F1000"/>
     <hyperlink r:id="rId955" ref="F1001"/>
     <hyperlink r:id="rId956" ref="F1002"/>
-    <hyperlink r:id="rId957" ref="F1003"/>
-    <hyperlink r:id="rId958" ref="F1004"/>
-    <hyperlink r:id="rId959" ref="F1005"/>
-    <hyperlink r:id="rId960" ref="F1006"/>
-    <hyperlink r:id="rId961" ref="F1007"/>
-    <hyperlink r:id="rId962" ref="F1008"/>
-    <hyperlink r:id="rId963" ref="F1009"/>
-    <hyperlink r:id="rId964" ref="F1010"/>
-    <hyperlink r:id="rId965" ref="F1011"/>
-    <hyperlink r:id="rId966" ref="F1012"/>
-    <hyperlink r:id="rId967" ref="F1013"/>
-    <hyperlink r:id="rId968" ref="F1014"/>
-    <hyperlink r:id="rId969" ref="F1015"/>
-    <hyperlink r:id="rId970" ref="F1016"/>
-    <hyperlink r:id="rId971" ref="F1017"/>
-    <hyperlink r:id="rId972" ref="F1018"/>
-    <hyperlink r:id="rId973" ref="F1019"/>
-    <hyperlink r:id="rId974" ref="F1020"/>
-    <hyperlink r:id="rId975" ref="F1021"/>
-    <hyperlink r:id="rId976" ref="F1022"/>
-    <hyperlink r:id="rId977" ref="F1023"/>
-    <hyperlink r:id="rId978" ref="F1024"/>
-    <hyperlink r:id="rId979" ref="F1025"/>
-    <hyperlink r:id="rId980" ref="F1026"/>
-    <hyperlink r:id="rId981" ref="F1027"/>
-    <hyperlink r:id="rId982" ref="F1028"/>
-    <hyperlink r:id="rId983" ref="F1029"/>
-    <hyperlink r:id="rId984" ref="F1030"/>
-    <hyperlink r:id="rId985" ref="F1031"/>
-    <hyperlink r:id="rId986" ref="F1032"/>
-    <hyperlink r:id="rId987" ref="F1033"/>
-    <hyperlink r:id="rId988" ref="F1034"/>
-    <hyperlink r:id="rId989" ref="F1035"/>
-    <hyperlink r:id="rId990" ref="F1036"/>
-    <hyperlink r:id="rId991" ref="F1037"/>
-    <hyperlink r:id="rId992" ref="F1038"/>
-    <hyperlink r:id="rId993" ref="F1039"/>
-    <hyperlink r:id="rId994" ref="F1040"/>
-    <hyperlink r:id="rId995" ref="F1041"/>
-    <hyperlink r:id="rId996" ref="F1042"/>
-    <hyperlink r:id="rId997" ref="F1043"/>
-    <hyperlink r:id="rId998" ref="F1044"/>
-    <hyperlink r:id="rId999" ref="F1045"/>
-    <hyperlink r:id="rId1000" ref="F1046"/>
-    <hyperlink r:id="rId1001" ref="F1047"/>
-    <hyperlink r:id="rId1002" ref="F1048"/>
-    <hyperlink r:id="rId1003" ref="F1049"/>
-    <hyperlink r:id="rId1004" ref="F1050"/>
-    <hyperlink r:id="rId1005" ref="F1051"/>
-    <hyperlink r:id="rId1006" ref="F1052"/>
-    <hyperlink r:id="rId1007" ref="F1053"/>
-    <hyperlink r:id="rId1008" ref="F1054"/>
-    <hyperlink r:id="rId1009" ref="F1055"/>
-    <hyperlink r:id="rId1010" ref="F1056"/>
+    <hyperlink r:id="rId957" ref="F1005"/>
+    <hyperlink r:id="rId958" ref="F1006"/>
+    <hyperlink r:id="rId959" ref="F1007"/>
+    <hyperlink r:id="rId960" ref="F1008"/>
+    <hyperlink r:id="rId961" ref="F1009"/>
+    <hyperlink r:id="rId962" ref="F1010"/>
+    <hyperlink r:id="rId963" ref="F1011"/>
+    <hyperlink r:id="rId964" ref="F1012"/>
+    <hyperlink r:id="rId965" ref="F1013"/>
+    <hyperlink r:id="rId966" ref="F1014"/>
+    <hyperlink r:id="rId967" ref="F1015"/>
+    <hyperlink r:id="rId968" ref="F1016"/>
+    <hyperlink r:id="rId969" ref="F1017"/>
+    <hyperlink r:id="rId970" ref="F1024"/>
+    <hyperlink r:id="rId971" ref="F1025"/>
+    <hyperlink r:id="rId972" ref="F1026"/>
+    <hyperlink r:id="rId973" ref="F1027"/>
+    <hyperlink r:id="rId974" ref="F1028"/>
+    <hyperlink r:id="rId975" ref="F1029"/>
+    <hyperlink r:id="rId976" ref="F1030"/>
+    <hyperlink r:id="rId977" ref="F1031"/>
+    <hyperlink r:id="rId978" ref="F1032"/>
+    <hyperlink r:id="rId979" ref="F1033"/>
+    <hyperlink r:id="rId980" ref="F1034"/>
+    <hyperlink r:id="rId981" ref="F1035"/>
+    <hyperlink r:id="rId982" ref="F1036"/>
+    <hyperlink r:id="rId983" ref="F1037"/>
+    <hyperlink r:id="rId984" ref="F1038"/>
+    <hyperlink r:id="rId985" ref="F1039"/>
+    <hyperlink r:id="rId986" ref="F1040"/>
+    <hyperlink r:id="rId987" ref="F1041"/>
+    <hyperlink r:id="rId988" ref="F1042"/>
+    <hyperlink r:id="rId989" ref="F1043"/>
+    <hyperlink r:id="rId990" ref="F1044"/>
+    <hyperlink r:id="rId991" ref="F1045"/>
+    <hyperlink r:id="rId992" ref="F1046"/>
+    <hyperlink r:id="rId993" ref="F1047"/>
+    <hyperlink r:id="rId994" ref="F1048"/>
+    <hyperlink r:id="rId995" ref="F1049"/>
+    <hyperlink r:id="rId996" ref="F1050"/>
+    <hyperlink r:id="rId997" ref="F1051"/>
+    <hyperlink r:id="rId998" ref="F1052"/>
+    <hyperlink r:id="rId999" ref="F1053"/>
+    <hyperlink r:id="rId1000" ref="F1054"/>
+    <hyperlink r:id="rId1001" ref="F1055"/>
+    <hyperlink r:id="rId1002" ref="F1056"/>
+    <hyperlink r:id="rId1003" ref="F1057"/>
+    <hyperlink r:id="rId1004" ref="F1058"/>
+    <hyperlink r:id="rId1005" ref="F1059"/>
+    <hyperlink r:id="rId1006" ref="F1060"/>
+    <hyperlink r:id="rId1007" ref="F1061"/>
+    <hyperlink r:id="rId1008" ref="F1062"/>
+    <hyperlink r:id="rId1009" ref="F1063"/>
+    <hyperlink r:id="rId1010" ref="F1064"/>
+    <hyperlink r:id="rId1011" ref="F1065"/>
+    <hyperlink r:id="rId1012" ref="F1066"/>
+    <hyperlink r:id="rId1013" ref="F1067"/>
+    <hyperlink r:id="rId1014" ref="F1068"/>
+    <hyperlink r:id="rId1015" ref="F1069"/>
+    <hyperlink r:id="rId1016" ref="F1070"/>
+    <hyperlink r:id="rId1017" ref="F1071"/>
+    <hyperlink r:id="rId1018" ref="F1072"/>
+    <hyperlink r:id="rId1019" ref="F1073"/>
+    <hyperlink r:id="rId1020" ref="F1074"/>
+    <hyperlink r:id="rId1021" ref="F1075"/>
+    <hyperlink r:id="rId1022" ref="F1076"/>
+    <hyperlink r:id="rId1023" ref="F1077"/>
+    <hyperlink r:id="rId1024" ref="F1078"/>
+    <hyperlink r:id="rId1025" ref="F1079"/>
+    <hyperlink r:id="rId1026" ref="F1080"/>
+    <hyperlink r:id="rId1027" ref="F1081"/>
+    <hyperlink r:id="rId1028" ref="F1082"/>
+    <hyperlink r:id="rId1029" ref="F1083"/>
+    <hyperlink r:id="rId1030" ref="F1084"/>
+    <hyperlink r:id="rId1031" ref="F1085"/>
+    <hyperlink r:id="rId1032" ref="F1086"/>
+    <hyperlink r:id="rId1033" ref="F1087"/>
+    <hyperlink r:id="rId1034" ref="F1088"/>
+    <hyperlink r:id="rId1035" ref="F1089"/>
+    <hyperlink r:id="rId1036" ref="F1090"/>
   </hyperlinks>
-  <drawing r:id="rId1011"/>
-  <legacyDrawing r:id="rId1012"/>
+  <drawing r:id="rId1037"/>
+  <legacyDrawing r:id="rId1038"/>
 </worksheet>
 </file>
 
@@ -56080,10 +57148,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="55" t="s">
-        <v>1157</v>
+        <v>1189</v>
       </c>
       <c r="F1" s="56" t="s">
-        <v>1158</v>
+        <v>1190</v>
       </c>
       <c r="G1" s="56"/>
       <c r="H1" s="56"/>
@@ -56092,7 +57160,7 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>1159</v>
+        <v>1191</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>24</v>
@@ -56142,7 +57210,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="F4" s="57" t="s">
-        <v>1160</v>
+        <v>1192</v>
       </c>
       <c r="G4" s="64">
         <v>0.01053725</v>
@@ -56188,7 +57256,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="F6" s="57" t="s">
-        <v>1161</v>
+        <v>1193</v>
       </c>
       <c r="G6" s="64"/>
       <c r="H6" s="64">
@@ -56211,7 +57279,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="F7" s="57" t="s">
-        <v>1162</v>
+        <v>1194</v>
       </c>
       <c r="G7" s="64">
         <v>0.01003394598214286</v>
@@ -56251,7 +57319,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="F9" s="57" t="s">
-        <v>1163</v>
+        <v>1195</v>
       </c>
       <c r="G9" s="64">
         <v>0.009942447023809527</v>
@@ -56308,7 +57376,7 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>1164</v>
+        <v>1196</v>
       </c>
       <c r="B12" s="9">
         <v>0.010118942412698416</v>
@@ -56320,7 +57388,7 @@
         <v>0.04156248611111111</v>
       </c>
       <c r="F12" s="57" t="s">
-        <v>1165</v>
+        <v>1197</v>
       </c>
       <c r="G12" s="64">
         <v>0.010359710714285717</v>
@@ -56420,10 +57488,10 @@
     </row>
     <row r="18">
       <c r="A18" s="65" t="s">
-        <v>1166</v>
+        <v>1198</v>
       </c>
       <c r="F18" s="66" t="s">
-        <v>1167</v>
+        <v>1199</v>
       </c>
       <c r="J18" s="57"/>
     </row>
@@ -56542,7 +57610,7 @@
         <v>0.135</v>
       </c>
       <c r="F23" s="74" t="s">
-        <v>1161</v>
+        <v>1193</v>
       </c>
       <c r="G23" s="79">
         <f>AVERAGE(H23/2,I23/3)</f>
@@ -56570,7 +57638,7 @@
         <v>0.3</v>
       </c>
       <c r="F24" s="74" t="s">
-        <v>1165</v>
+        <v>1197</v>
       </c>
       <c r="G24" s="79">
         <v>0.010359710714285717</v>
@@ -56598,7 +57666,7 @@
         <v>0.3</v>
       </c>
       <c r="F25" s="74" t="s">
-        <v>1162</v>
+        <v>1194</v>
       </c>
       <c r="G25" s="79">
         <v>0.01003394598214286</v>
@@ -56656,7 +57724,7 @@
         <v>0.135</v>
       </c>
       <c r="F27" s="74" t="s">
-        <v>1163</v>
+        <v>1195</v>
       </c>
       <c r="G27" s="79">
         <v>0.009942447023809527</v>
@@ -56766,7 +57834,7 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>1168</v>
+        <v>1200</v>
       </c>
       <c r="C33" s="9"/>
       <c r="F33" s="57"/>
@@ -64551,7 +65619,7 @@
   <sheetData>
     <row r="1">
       <c r="D1" s="3" t="s">
-        <v>1170</v>
+        <v>1202</v>
       </c>
       <c r="E1" s="47"/>
     </row>
@@ -64711,7 +65779,7 @@
         <v>u/DellEnableUnderClock 0.02 damo</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>1172</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="28">
@@ -64721,7 +65789,7 @@
       </c>
       <c r="H28" s="85"/>
       <c r="I28" s="86" t="s">
-        <v>1174</v>
+        <v>1206</v>
       </c>
       <c r="J28" s="85"/>
       <c r="K28" s="85"/>
@@ -65026,7 +66094,7 @@
     </row>
     <row r="62">
       <c r="D62" s="3" t="s">
-        <v>1175</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="63">
@@ -66554,228 +67622,205 @@
     <row r="365">
       <c r="D365" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>AlgoRhythMatic 0.07 damo</v>
       </c>
     </row>
     <row r="366">
       <c r="D366" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>Blessed4aDay 0.03 damo</v>
       </c>
     </row>
     <row r="367">
       <c r="D367" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>DingusMungus  0.03 damo</v>
       </c>
     </row>
     <row r="368">
       <c r="D368" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>Grinnmarr 0.06 damo</v>
       </c>
     </row>
     <row r="369">
       <c r="D369" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>kerrilija 0.03 damo</v>
       </c>
     </row>
     <row r="370">
       <c r="D370" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>mochanerd 0.06 damo</v>
       </c>
     </row>
     <row r="371">
       <c r="D371" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>moloch10 0.06 damo</v>
       </c>
     </row>
     <row r="372">
       <c r="D372" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>motuwagon  0.03 damo</v>
       </c>
     </row>
     <row r="373">
       <c r="D373" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>robbie 0.09 damo</v>
       </c>
     </row>
     <row r="374">
       <c r="D374" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>uberg33k 0.04 damo</v>
       </c>
     </row>
     <row r="375">
       <c r="D375" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>UncleDooom 0.03 damo</v>
       </c>
     </row>
     <row r="376">
-      <c r="C376" s="83"/>
       <c r="D376" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v> 0.53 damo</v>
       </c>
     </row>
     <row r="377">
-      <c r="C377" s="83"/>
       <c r="D377" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>akpepe 0.03 damo</v>
       </c>
     </row>
     <row r="378">
-      <c r="C378" s="83"/>
       <c r="D378" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>AlgoRhythMatic 0.07 damo</v>
       </c>
     </row>
     <row r="379">
-      <c r="C379" s="83"/>
       <c r="D379" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>Algoworm  0.03 damo</v>
       </c>
     </row>
     <row r="380">
-      <c r="C380" s="83"/>
       <c r="D380" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>dankster1  0.03 damo</v>
       </c>
     </row>
     <row r="381">
-      <c r="C381" s="83"/>
       <c r="D381" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>fifthrace  0.06 damo</v>
       </c>
     </row>
     <row r="382">
-      <c r="C382" s="83"/>
       <c r="D382" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>Grinnmarr 0.14 damo</v>
       </c>
     </row>
     <row r="383">
-      <c r="C383" s="83"/>
       <c r="D383" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>kerrilija 0.23 damo</v>
       </c>
     </row>
     <row r="384">
-      <c r="C384" s="83"/>
       <c r="D384" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>leaf 🍃 0.03 damo</v>
       </c>
     </row>
     <row r="385">
-      <c r="C385" s="83"/>
       <c r="D385" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>Max 0.03 damo</v>
       </c>
     </row>
     <row r="386">
-      <c r="C386" s="83"/>
       <c r="D386" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>mochanerd 0.14 damo</v>
       </c>
     </row>
     <row r="387">
-      <c r="C387" s="83"/>
       <c r="D387" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v> 0.78 damo</v>
       </c>
     </row>
     <row r="388">
-      <c r="C388" s="83"/>
       <c r="D388" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="389">
-      <c r="C389" s="83"/>
       <c r="D389" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="390">
-      <c r="C390" s="83"/>
       <c r="D390" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="391">
-      <c r="C391" s="83"/>
       <c r="D391" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="392">
-      <c r="C392" s="83"/>
       <c r="D392" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="393">
-      <c r="C393" s="83"/>
       <c r="D393" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="394">
-      <c r="C394" s="83"/>
       <c r="D394" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="395">
-      <c r="C395" s="83"/>
       <c r="D395" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="396">
-      <c r="C396" s="83"/>
       <c r="D396" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="397">
-      <c r="C397" s="83"/>
       <c r="D397" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="398">
-      <c r="C398" s="83"/>
       <c r="D398" s="5" t="str">
         <f t="shared" si="8"/>
-        <v> 0 damo</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="399">

</xml_diff>